<commit_message>
authors_book.xlsx par ordre alphabetique
</commit_message>
<xml_diff>
--- a/authors_book.xlsx
+++ b/authors_book.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="authors" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Authors" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,75 +422,59 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" t="n">
-        <v>1</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Albert Einstein</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>André Gide</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Eleanor Roosevelt</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>J.K. Rowling</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jane Austen</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Marilyn Monroe</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Steve Martin</t>
+        </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Thomas A. Edison</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>